<commit_message>
more roads to lord
</commit_message>
<xml_diff>
--- a/roads-to-lord/checklist.xlsx
+++ b/roads-to-lord/checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/roads-to-lord/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3517BCB-FE3E-C448-B85A-358FA0D6B219}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F9512D-054A-D745-A5FC-FCE3C159AEDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{4E82693C-2977-0843-AF60-B42AA7500F20}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{4E82693C-2977-0843-AF60-B42AA7500F20}"/>
   </bookViews>
   <sheets>
     <sheet name="checklist" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
   <si>
     <t>year</t>
   </si>
@@ -174,6 +174,27 @@
   </si>
   <si>
     <t>supplement</t>
+  </si>
+  <si>
+    <t>ビヨンド・ローズ・トゥ・ロードでわかる実践RPG入門</t>
+  </si>
+  <si>
+    <t>精霊の大地―ビヨンド・ローズ・トゥ・ロードでわかる実践RPG入門 2</t>
+  </si>
+  <si>
+    <t>BNN</t>
+  </si>
+  <si>
+    <t>beyond_roads_to_lord_primer1.jpg</t>
+  </si>
+  <si>
+    <t>beyond_roads_to_lord_primer2.jpg</t>
+  </si>
+  <si>
+    <t>A practical introduction to RPGs by means of Beyond Roads to Lord</t>
+  </si>
+  <si>
+    <t>Earth Spirits: A practical introduction to RPGs by means of Beyond Roads to Lord Vol 2</t>
   </si>
 </sst>
 </file>
@@ -540,16 +561,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A06371B-2BD0-8F4B-BDBA-C0727628F293}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="69.6640625" customWidth="1"/>
-    <col min="3" max="3" width="48.83203125" customWidth="1"/>
+    <col min="3" max="3" width="61.33203125" customWidth="1"/>
     <col min="4" max="4" width="23.1640625" customWidth="1"/>
     <col min="5" max="5" width="32.33203125" customWidth="1"/>
   </cols>
@@ -804,6 +825,46 @@
         <v>14</v>
       </c>
       <c r="F14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1991</v>
+      </c>
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1991</v>
+      </c>
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
roads to lord dates
</commit_message>
<xml_diff>
--- a/roads-to-lord/checklist.xlsx
+++ b/roads-to-lord/checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/roads-to-lord/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Source/japanese-collectors-list/roads-to-lord/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABCF746-11FA-9E4D-9544-29C9EE534B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCEA7ECD-79E6-7F46-BD1D-DECD9862A1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{4E82693C-2977-0843-AF60-B42AA7500F20}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="25480" windowHeight="16340" xr2:uid="{4E82693C-2977-0843-AF60-B42AA7500F20}"/>
   </bookViews>
   <sheets>
     <sheet name="checklist" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="96">
   <si>
     <t>year</t>
   </si>
@@ -152,12 +152,6 @@
     <t>product_type</t>
   </si>
   <si>
-    <t>ローズ・トゥ・ロード拡張キット ストラディウム編 デラックスセット</t>
-  </si>
-  <si>
-    <t>Stra Diumn: Roads to Lord Expansion Kit Deluxe Set</t>
-  </si>
-  <si>
     <t>stra_diumn_1.jpg</t>
   </si>
   <si>
@@ -167,12 +161,6 @@
     <t>box set</t>
   </si>
   <si>
-    <t>ローズ・トゥ・ロード拡張キット ストラディウム編 Vol.2</t>
-  </si>
-  <si>
-    <t>Stra Diumn: Roads to Lord Expansion Kit</t>
-  </si>
-  <si>
     <t>supplement</t>
   </si>
   <si>
@@ -267,6 +255,72 @@
   </si>
   <si>
     <t>Enterbrain</t>
+  </si>
+  <si>
+    <t>ローズ・トゥ・ロード拡張キット ストラディウム編 Vol. 1</t>
+  </si>
+  <si>
+    <t>product_code</t>
+  </si>
+  <si>
+    <t>stra_diumn_3.jpg</t>
+  </si>
+  <si>
+    <t>Stra Diumn: Roads to Lord Expansion Kit Vol. 1</t>
+  </si>
+  <si>
+    <t>Stra Diumn: Roads to Lord Expansion Kit Vol. 2</t>
+  </si>
+  <si>
+    <t>Stra Diumn: Roads to Lord Expansion Kit Vol. 3</t>
+  </si>
+  <si>
+    <t>ローズ・トゥ・ロード拡張キット ストラディウム編 Vol. 2</t>
+  </si>
+  <si>
+    <t>ローズ・トゥ・ロード拡張キット ストラディウム編 Vol. 3</t>
+  </si>
+  <si>
+    <t>HG-030R</t>
+  </si>
+  <si>
+    <t>HG-051R</t>
+  </si>
+  <si>
+    <t>HG-062R-1</t>
+  </si>
+  <si>
+    <t>HG-062R-2</t>
+  </si>
+  <si>
+    <t>HG-062R-3</t>
+  </si>
+  <si>
+    <t>HG-042R</t>
+  </si>
+  <si>
+    <t>Yuentai</t>
+  </si>
+  <si>
+    <t>Y-8901</t>
+  </si>
+  <si>
+    <t>Y-9002</t>
+  </si>
+  <si>
+    <t>Y-9306</t>
+  </si>
+  <si>
+    <t>Y-9601</t>
+  </si>
+  <si>
+    <t>Y-9405</t>
+  </si>
+  <si>
+    <t>Y-9403</t>
+  </si>
+  <si>
+    <t>Y-9402</t>
   </si>
 </sst>
 </file>
@@ -633,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A06371B-2BD0-8F4B-BDBA-C0727628F293}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="A18" sqref="A18:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -647,7 +701,7 @@
     <col min="5" max="5" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -666,8 +720,11 @@
       <c r="F1" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1984</v>
       </c>
@@ -684,393 +741,461 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="G2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1985</v>
+      </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="G3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1986</v>
+      </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
       </c>
       <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
         <v>41</v>
       </c>
-      <c r="F4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1987</v>
+      </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="G5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>1985</v>
+        <v>1987</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="G6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>1989</v>
+        <v>1987</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>79</v>
       </c>
       <c r="D7" t="s">
         <v>15</v>
       </c>
       <c r="E7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1989</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" t="s">
         <v>5</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1991</v>
+      </c>
+      <c r="B10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="C10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1991</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>1993</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B12" t="s">
         <v>25</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C12" t="s">
         <v>26</v>
       </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="D12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" t="s">
         <v>27</v>
       </c>
-      <c r="F9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+      <c r="F12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
         <v>36</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C13" t="s">
         <v>37</v>
       </c>
-      <c r="D10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="D13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" t="s">
         <v>6</v>
       </c>
-      <c r="F10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
+      <c r="F13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
         <v>34</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C14" t="s">
         <v>35</v>
       </c>
-      <c r="D11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="D14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E14" t="s">
         <v>7</v>
       </c>
-      <c r="F11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
+      <c r="F14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
         <v>30</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C15" t="s">
         <v>31</v>
       </c>
-      <c r="D12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="D15" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" t="s">
         <v>9</v>
       </c>
-      <c r="F12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
+      <c r="F15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
         <v>28</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C16" t="s">
         <v>29</v>
       </c>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="D16" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" t="s">
         <v>10</v>
       </c>
-      <c r="F13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
+      <c r="F16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
         <v>33</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C17" t="s">
         <v>32</v>
       </c>
-      <c r="D14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="D17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" t="s">
         <v>14</v>
       </c>
-      <c r="F14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>1991</v>
-      </c>
-      <c r="B15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="F17" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2002</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" t="s">
         <v>52</v>
       </c>
-      <c r="D15" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" t="s">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2006</v>
+      </c>
+      <c r="B23" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2010</v>
+      </c>
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" t="s">
         <v>50</v>
       </c>
-      <c r="F15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>1991</v>
-      </c>
-      <c r="B16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="D24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" t="s">
         <v>51</v>
       </c>
-      <c r="F16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>68</v>
-      </c>
-      <c r="C17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" t="s">
-        <v>71</v>
-      </c>
-      <c r="E17" t="s">
-        <v>70</v>
-      </c>
-      <c r="F17" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>2002</v>
-      </c>
-      <c r="B18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" t="s">
-        <v>57</v>
-      </c>
-      <c r="F18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" t="s">
-        <v>61</v>
-      </c>
-      <c r="F19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20" t="s">
-        <v>67</v>
-      </c>
-      <c r="F20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
-        <v>64</v>
-      </c>
-      <c r="C21" t="s">
-        <v>66</v>
-      </c>
-      <c r="D21" t="s">
-        <v>60</v>
-      </c>
-      <c r="E21" t="s">
-        <v>65</v>
-      </c>
-      <c r="F21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>2006</v>
-      </c>
-      <c r="B22" t="s">
-        <v>73</v>
-      </c>
-      <c r="C22" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E22" t="s">
-        <v>76</v>
-      </c>
-      <c r="F22" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>2010</v>
-      </c>
-      <c r="B23" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" t="s">
-        <v>77</v>
-      </c>
-      <c r="E23" t="s">
-        <v>55</v>
-      </c>
-      <c r="F23" t="s">
-        <v>56</v>
+      <c r="F24" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E14">
-    <sortCondition ref="A3:A14"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G8">
+    <sortCondition ref="A2:A8"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>